<commit_message>
tweet_fetcher extended with query string searching
</commit_message>
<xml_diff>
--- a/src/performance_testing/no_comment_performance.xlsx
+++ b/src/performance_testing/no_comment_performance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="length_dast" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="24">
   <si>
     <t>model</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>dastpheme_majority_nts</t>
+  </si>
+  <si>
+    <t>Pheme</t>
   </si>
 </sst>
 </file>
@@ -1008,11 +1011,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="425969056"/>
-        <c:axId val="425970624"/>
+        <c:axId val="557124536"/>
+        <c:axId val="557124928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425969056"/>
+        <c:axId val="557124536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1058,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425970624"/>
+        <c:crossAx val="557124928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1063,7 +1066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425970624"/>
+        <c:axId val="557124928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1117,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425969056"/>
+        <c:crossAx val="557124536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1235,7 +1238,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1336,7 +1338,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1480,7 +1481,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1570,11 +1570,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571770080"/>
-        <c:axId val="571768120"/>
+        <c:axId val="557101800"/>
+        <c:axId val="557106896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571770080"/>
+        <c:axId val="557101800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1617,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571768120"/>
+        <c:crossAx val="557106896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1625,7 +1625,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571768120"/>
+        <c:axId val="557106896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1676,7 +1676,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571770080"/>
+        <c:crossAx val="557101800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1690,7 +1690,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1797,7 +1796,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1898,7 +1896,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2042,7 +2039,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2132,11 +2128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571770472"/>
-        <c:axId val="571766160"/>
+        <c:axId val="557102192"/>
+        <c:axId val="557094744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571770472"/>
+        <c:axId val="557102192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2179,7 +2175,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571766160"/>
+        <c:crossAx val="557094744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2187,7 +2183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571766160"/>
+        <c:axId val="557094744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2238,7 +2234,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571770472"/>
+        <c:crossAx val="557102192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2252,7 +2248,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2359,7 +2354,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2460,7 +2454,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2604,7 +2597,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2694,11 +2686,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571767728"/>
-        <c:axId val="571773608"/>
+        <c:axId val="557102584"/>
+        <c:axId val="557119048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571767728"/>
+        <c:axId val="557102584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2741,7 +2733,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571773608"/>
+        <c:crossAx val="557119048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2749,7 +2741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571773608"/>
+        <c:axId val="557119048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2800,7 +2792,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571767728"/>
+        <c:crossAx val="557102584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2814,7 +2806,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2921,7 +2912,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3022,7 +3012,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3166,7 +3155,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3256,11 +3244,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571771256"/>
-        <c:axId val="571771648"/>
+        <c:axId val="557119440"/>
+        <c:axId val="557108072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571771256"/>
+        <c:axId val="557119440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3303,7 +3291,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571771648"/>
+        <c:crossAx val="557108072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3311,7 +3299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571771648"/>
+        <c:axId val="557108072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3362,7 +3350,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571771256"/>
+        <c:crossAx val="557119440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3376,7 +3364,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3818,11 +3805,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571772824"/>
-        <c:axId val="571774000"/>
+        <c:axId val="557110032"/>
+        <c:axId val="557110424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571772824"/>
+        <c:axId val="557110032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3865,7 +3852,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571774000"/>
+        <c:crossAx val="557110424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3873,7 +3860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571774000"/>
+        <c:axId val="557110424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3924,7 +3911,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571772824"/>
+        <c:crossAx val="557110032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4380,11 +4367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571762632"/>
-        <c:axId val="571763808"/>
+        <c:axId val="557112776"/>
+        <c:axId val="557113168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571762632"/>
+        <c:axId val="557112776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4427,7 +4414,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571763808"/>
+        <c:crossAx val="557113168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4435,7 +4422,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571763808"/>
+        <c:axId val="557113168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4486,7 +4473,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571762632"/>
+        <c:crossAx val="557112776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4942,11 +4929,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571758712"/>
-        <c:axId val="571759496"/>
+        <c:axId val="557117088"/>
+        <c:axId val="557107288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571758712"/>
+        <c:axId val="557117088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4989,7 +4976,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571759496"/>
+        <c:crossAx val="557107288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4997,7 +4984,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571759496"/>
+        <c:axId val="557107288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5048,7 +5035,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571758712"/>
+        <c:crossAx val="557117088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5504,11 +5491,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571748912"/>
-        <c:axId val="571739504"/>
+        <c:axId val="557110816"/>
+        <c:axId val="557107680"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571748912"/>
+        <c:axId val="557110816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5551,7 +5538,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571739504"/>
+        <c:crossAx val="557107680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5559,7 +5546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571739504"/>
+        <c:axId val="557107680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5610,7 +5597,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571748912"/>
+        <c:crossAx val="557110816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6032,11 +6019,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="186010704"/>
-        <c:axId val="186007960"/>
+        <c:axId val="557111208"/>
+        <c:axId val="557117480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186010704"/>
+        <c:axId val="557111208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6079,7 +6066,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186007960"/>
+        <c:crossAx val="557117480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6087,7 +6074,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186007960"/>
+        <c:axId val="557117480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6138,7 +6125,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186010704"/>
+        <c:crossAx val="557111208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6560,11 +6547,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="186009136"/>
-        <c:axId val="186009528"/>
+        <c:axId val="557115128"/>
+        <c:axId val="557108464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186009136"/>
+        <c:axId val="557115128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6607,7 +6594,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186009528"/>
+        <c:crossAx val="557108464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6615,7 +6602,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186009528"/>
+        <c:axId val="557108464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6666,7 +6653,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186009136"/>
+        <c:crossAx val="557115128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7122,11 +7109,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="425963960"/>
-        <c:axId val="425965136"/>
+        <c:axId val="557103368"/>
+        <c:axId val="557095528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425963960"/>
+        <c:axId val="557103368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7169,7 +7156,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425965136"/>
+        <c:crossAx val="557095528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7177,7 +7164,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425965136"/>
+        <c:axId val="557095528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7228,7 +7215,535 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425963960"/>
+        <c:crossAx val="557103368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dataset_comparison!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>f1_macro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="da-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dataset_comparison!$A$36:$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>pheme</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dast</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dast_majority</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pheme_majority</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dastpheme_majority</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dast_ts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dataset_comparison!$B$36:$B$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dataset_comparison!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="da-DK"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dataset_comparison!$A$36:$A$44</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>pheme</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>dastpheme</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>dast</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>dast_majority</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>pheme_majority</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>dastpheme_majority</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>pheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>dastpheme_ts</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>dast_ts</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dataset_comparison!$C$36:$C$44</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="552579936"/>
+        <c:axId val="552581896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="552579936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552581896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="552581896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="552579936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7684,11 +8199,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="425964744"/>
-        <c:axId val="425968664"/>
+        <c:axId val="557095920"/>
+        <c:axId val="557096704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="425964744"/>
+        <c:axId val="557095920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7731,7 +8246,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425968664"/>
+        <c:crossAx val="557096704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7739,7 +8254,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425968664"/>
+        <c:axId val="557096704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7790,7 +8305,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425964744"/>
+        <c:crossAx val="557095920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8246,11 +8761,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="186200336"/>
-        <c:axId val="186196024"/>
+        <c:axId val="557097096"/>
+        <c:axId val="557099056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186200336"/>
+        <c:axId val="557097096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8293,7 +8808,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186196024"/>
+        <c:crossAx val="557099056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8301,7 +8816,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186196024"/>
+        <c:axId val="557099056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8352,7 +8867,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186200336"/>
+        <c:crossAx val="557097096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8808,11 +9323,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="186196808"/>
-        <c:axId val="186194848"/>
+        <c:axId val="557101408"/>
+        <c:axId val="557098272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186196808"/>
+        <c:axId val="557101408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8855,7 +9370,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186194848"/>
+        <c:crossAx val="557098272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8863,7 +9378,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186194848"/>
+        <c:axId val="557098272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8914,7 +9429,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186196808"/>
+        <c:crossAx val="557101408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9370,11 +9885,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="186201120"/>
-        <c:axId val="186200728"/>
+        <c:axId val="557101016"/>
+        <c:axId val="557102976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186201120"/>
+        <c:axId val="557101016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9417,7 +9932,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186200728"/>
+        <c:crossAx val="557102976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9425,7 +9940,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186200728"/>
+        <c:axId val="557102976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9476,7 +9991,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186201120"/>
+        <c:crossAx val="557101016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9597,7 +10112,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9698,7 +10212,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9842,7 +10355,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -9932,11 +10444,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="571750872"/>
-        <c:axId val="571751264"/>
+        <c:axId val="557106112"/>
+        <c:axId val="557098664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="571750872"/>
+        <c:axId val="557106112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9979,7 +10491,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571751264"/>
+        <c:crossAx val="557098664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9987,7 +10499,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571751264"/>
+        <c:axId val="557098664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10038,7 +10550,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="571750872"/>
+        <c:crossAx val="557106112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10052,7 +10564,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10159,7 +10670,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10260,7 +10770,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10404,7 +10913,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10494,11 +11002,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="508302920"/>
-        <c:axId val="508304488"/>
+        <c:axId val="557106504"/>
+        <c:axId val="557099448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="508302920"/>
+        <c:axId val="557106504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10541,7 +11049,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508304488"/>
+        <c:crossAx val="557099448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10549,7 +11057,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="508304488"/>
+        <c:axId val="557099448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10600,7 +11108,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="508302920"/>
+        <c:crossAx val="557106504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10614,7 +11122,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10721,7 +11228,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10822,7 +11328,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -10966,7 +11471,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -11056,11 +11560,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="186012272"/>
-        <c:axId val="186007568"/>
+        <c:axId val="557100232"/>
+        <c:axId val="557095136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="186012272"/>
+        <c:axId val="557100232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11103,7 +11607,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186007568"/>
+        <c:crossAx val="557095136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11111,7 +11615,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="186007568"/>
+        <c:axId val="557095136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11162,7 +11666,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="186012272"/>
+        <c:crossAx val="557100232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11176,7 +11680,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11723,6 +12226,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors20.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -17559,6 +18102,511 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style20.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -22216,6 +23264,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -22484,7 +23564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -24323,10 +25403,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24564,6 +25644,121 @@
         <v>0.81</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C36">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="C37">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="C38">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>0.45</v>
+      </c>
+      <c r="C39">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40">
+        <v>0.45</v>
+      </c>
+      <c r="C40">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41">
+        <v>0.45</v>
+      </c>
+      <c r="C41">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>0.5</v>
+      </c>
+      <c r="C42">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>0.47</v>
+      </c>
+      <c r="C43">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>0.47</v>
+      </c>
+      <c r="C44">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>